<commit_message>
add coloumn otp codes
</commit_message>
<xml_diff>
--- a/public/template_alumni.xlsx
+++ b/public/template_alumni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_TracerStudy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDB4784-CFCA-4120-94B6-743D92AB7D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16382E7-E79C-4F17-9DAD-D7EDB71DADCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>NIM</t>
   </si>
@@ -48,28 +48,43 @@
     <t>S2 MRTI</t>
   </si>
   <si>
-    <t>Mahasiswa 1</t>
-  </si>
-  <si>
-    <t>Mahasiswa 3</t>
-  </si>
-  <si>
-    <t>Mahasiswa 4</t>
-  </si>
-  <si>
     <t>D4 Teknik Informatika</t>
   </si>
   <si>
     <t>D4 Sistem Informasi Bisnis</t>
   </si>
   <si>
-    <t>Mahasiswa 2</t>
-  </si>
-  <si>
     <t>Program_Studi</t>
   </si>
   <si>
     <t>Tanggal_Lulus</t>
+  </si>
+  <si>
+    <t>Kode_OTP</t>
+  </si>
+  <si>
+    <t>Doni Hermawan</t>
+  </si>
+  <si>
+    <t>Susila Rena Guvi</t>
+  </si>
+  <si>
+    <t>Bli Kusuma Wirawan</t>
+  </si>
+  <si>
+    <t>Vei Dorothea</t>
+  </si>
+  <si>
+    <t>DH23</t>
+  </si>
+  <si>
+    <t>SR24</t>
+  </si>
+  <si>
+    <t>BK25</t>
+  </si>
+  <si>
+    <t>VD26</t>
   </si>
 </sst>
 </file>
@@ -349,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3DBB98-3F9B-4BC6-B179-EC7FF714CC62}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -361,11 +376,12 @@
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -374,62 +390,77 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>1731710101</v>
+        <v>2341760123</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
         <v>44041</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>1731710102</v>
+        <v>2341760124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
         <v>44041</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1731710103</v>
+        <v>2341760125</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
         <v>44041</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1731710104</v>
+        <v>2341760126</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
         <v>44053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
send kode otp to email and revisi 27 mei
</commit_message>
<xml_diff>
--- a/public/template_alumni.xlsx
+++ b/public/template_alumni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_TracerStudy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16382E7-E79C-4F17-9DAD-D7EDB71DADCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA6773D-B1B3-42EB-864D-2082F8AB45DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Tanggal_Lulus</t>
   </si>
   <si>
-    <t>Kode_OTP</t>
-  </si>
-  <si>
     <t>Doni Hermawan</t>
   </si>
   <si>
@@ -75,16 +72,19 @@
     <t>Vei Dorothea</t>
   </si>
   <si>
-    <t>DH23</t>
-  </si>
-  <si>
-    <t>SR24</t>
-  </si>
-  <si>
-    <t>BK25</t>
-  </si>
-  <si>
-    <t>VD26</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>arindrakeysha@gmail.com</t>
+  </si>
+  <si>
+    <t>cascanekeysha@gmail.com</t>
+  </si>
+  <si>
+    <t>dekuw85@gmail.com</t>
+  </si>
+  <si>
+    <t>dinarullailil26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,6 +121,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,18 +146,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,7 +377,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,7 +400,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
@@ -404,9 +414,9 @@
         <v>2341760123</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1">
@@ -421,9 +431,9 @@
         <v>2341760124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="1">
@@ -438,9 +448,9 @@
         <v>2341760125</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1">
@@ -455,9 +465,9 @@
         <v>2341760126</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1">
@@ -465,6 +475,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{21B3E641-1365-4DC2-AE6D-2926426C7ECF}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{56553316-FDE7-46CE-ACCC-042A32185255}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{FA4B0C49-D9EE-4476-A0FC-9DC1FEB804D9}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{CE382C15-F757-4163-A4AF-B8D3EAC7F099}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>